<commit_message>
Fix some bug in Road Catalog
</commit_message>
<xml_diff>
--- a/conf/excel/C_Pedestrian.xlsx
+++ b/conf/excel/C_Pedestrian.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\长期文件\学习资料\综合学习资料\tencent\配置文件相关\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B313BB-B4A2-4662-A68B-5B2D0B206F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EC9F46-D762-4E85-B413-90CE4F6D8E25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="2700" windowWidth="23580" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11250" yWindow="5115" windowWidth="23580" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C_Pedestrian.conf" sheetId="1" r:id="rId1"/>
@@ -166,27 +166,9 @@
     <t>地下通道台阶</t>
   </si>
   <si>
-    <t>facility_type=04;type=00 || type=05 || type=07</t>
-  </si>
-  <si>
-    <t>facility_type=04;type=02 || type=03 || type=06</t>
-  </si>
-  <si>
-    <t>facility_type=03;type=00 || type=05 || type=07</t>
-  </si>
-  <si>
-    <t>facility_type=03;type=02 || type=03 || type=06</t>
-  </si>
-  <si>
-    <t>facility_type=05;type=00 || type=05 || type=07</t>
-  </si>
-  <si>
     <t>立体连接路平面</t>
   </si>
   <si>
-    <t>facility_type=05;type=02 || type=03 || type=06</t>
-  </si>
-  <si>
     <t>立体连接路台阶</t>
   </si>
   <si>
@@ -194,6 +176,30 @@
   </si>
   <si>
     <t>其他</t>
+  </si>
+  <si>
+    <t>facility_type=04;(type%=%00 || type%=%05 || type%=%07)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>facility_type=04;(type%=%02 || type%=%03 || type%=%06)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>facility_type=03;(type%=%00 || type%=%05 || type%=%07)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>facility_type=03;(type%=%02 || type%=%03 || type%=%06)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>facility_type=05;(type%=%00 || type%=%05 || type%=%07)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>facility_type=05;(type%=%02 || type%=%03 || type%=%06)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -563,7 +569,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B27" sqref="B26:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -644,7 +650,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
@@ -655,7 +661,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -666,7 +672,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
@@ -677,7 +683,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>15</v>
@@ -688,33 +694,33 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>